<commit_message>
daily test level 조정
</commit_message>
<xml_diff>
--- a/main/DB/UserList.xlsx
+++ b/main/DB/UserList.xlsx
@@ -104,13 +104,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +525,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="21" customHeight="1">
+    <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>ad1</t>
@@ -553,7 +553,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="3" ht="21" customHeight="1">
+    <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="4" t="inlineStr">
         <is>
           <t>ad2</t>
@@ -581,7 +581,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="4" ht="21" customHeight="1">
+    <row r="4" ht="19.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
         <is>
           <t>ad3</t>
@@ -609,7 +609,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="5" ht="21" customHeight="1">
+    <row r="5" ht="19.5" customHeight="1">
       <c r="A5" s="4" t="inlineStr">
         <is>
           <t>user1</t>
@@ -631,13 +631,13 @@
         </is>
       </c>
       <c r="E5" s="5" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>25569.3752959375</v>
-      </c>
-    </row>
-    <row r="6" ht="21" customHeight="1">
+        <v>45438</v>
+      </c>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>user2</t>
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="E6" s="5" t="n">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>45438</v>
       </c>
     </row>
-    <row r="7" ht="21" customHeight="1">
+    <row r="7" ht="19.5" customHeight="1">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>user3</t>
@@ -693,7 +693,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="8" ht="21" customHeight="1">
+    <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>user4</t>
@@ -721,7 +721,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1">
+    <row r="9" ht="19.5" customHeight="1">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>user5</t>
@@ -749,7 +749,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="10" ht="21" customHeight="1">
+    <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>user6</t>
@@ -777,7 +777,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="11" ht="21" customHeight="1">
+    <row r="11" ht="19.5" customHeight="1">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>user7</t>
@@ -805,7 +805,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="12" ht="21" customHeight="1">
+    <row r="12" ht="19.5" customHeight="1">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>user8</t>
@@ -833,7 +833,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="13" ht="21" customHeight="1">
+    <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="4" t="inlineStr">
         <is>
           <t>user9</t>
@@ -861,7 +861,7 @@
         <v>25569.3752959375</v>
       </c>
     </row>
-    <row r="14" ht="21" customHeight="1">
+    <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="4" t="inlineStr">
         <is>
           <t>user10</t>

</xml_diff>